<commit_message>
modif transport et graphique avec groupes de couleurs
</commit_message>
<xml_diff>
--- a/Models/Prospective_conso/data/Hypotheses_Transport_1D.xlsx
+++ b/Models/Prospective_conso/data/Hypotheses_Transport_1D.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin.girard/Documents/Code/Etude/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E3C602-5B2E-3B41-9772-95ACA571B54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E13D02B-AF35-8141-BBEB-836DFE5AFCCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3940" yWindow="1400" windowWidth="39920" windowHeight="21060" activeTab="4" xr2:uid="{F50204B1-83F4-DA42-A3C5-0BBDF8372860}"/>
+    <workbookView xWindow="11280" yWindow="5800" windowWidth="39920" windowHeight="21060" activeTab="3" xr2:uid="{F50204B1-83F4-DA42-A3C5-0BBDF8372860}"/>
   </bookViews>
   <sheets>
     <sheet name="0D" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="38">
   <si>
     <t>Nom</t>
   </si>
@@ -105,9 +105,6 @@
     <t>date_fin</t>
   </si>
   <si>
-    <t>retrofit_change_total_proportion_surface</t>
-  </si>
-  <si>
     <t>retrofit_change_total_proportion_Mds_voy_km</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>Rail court</t>
+  </si>
+  <si>
+    <t>aerien_international</t>
   </si>
 </sst>
 </file>
@@ -219,7 +219,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -255,17 +255,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -362,7 +351,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -373,20 +362,17 @@
     <xf numFmtId="2" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -708,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{779B33ED-9EE9-BB48-B4CA-335F6E62A50A}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -728,7 +714,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B2">
@@ -736,7 +722,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B3">
@@ -744,19 +730,11 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B4">
         <v>2050</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -781,15 +759,15 @@
       <c r="A1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>23</v>
+      <c r="B1" s="16" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2020</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="16">
         <v>0</v>
       </c>
     </row>
@@ -797,7 +775,7 @@
       <c r="A3">
         <v>2022</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="16">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
@@ -805,7 +783,7 @@
       <c r="A4">
         <v>2025</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="16">
         <v>0.1</v>
       </c>
     </row>
@@ -813,7 +791,7 @@
       <c r="A5">
         <v>2030</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="16">
         <v>0.35</v>
       </c>
     </row>
@@ -821,7 +799,7 @@
       <c r="A6">
         <v>2035</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="16">
         <v>0.7</v>
       </c>
     </row>
@@ -829,7 +807,7 @@
       <c r="A7">
         <v>2040</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="16">
         <v>0.85</v>
       </c>
     </row>
@@ -837,7 +815,7 @@
       <c r="A8">
         <v>2045</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="16">
         <v>0.95</v>
       </c>
     </row>
@@ -845,7 +823,7 @@
       <c r="A9">
         <v>2050</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="16">
         <v>1</v>
       </c>
     </row>
@@ -859,7 +837,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -869,40 +847,40 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2">
         <v>2020</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>2020</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>2020</v>
@@ -924,29 +902,29 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6">
         <v>2035</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>2035</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8">
         <v>2035</v>
@@ -968,29 +946,29 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10">
         <v>2050</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>2050</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12">
         <v>2050</v>
@@ -1017,10 +995,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9039F29E-2202-544B-A034-316D6E6A18F0}">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1029,48 +1007,46 @@
     <col min="3" max="3" width="21.5" customWidth="1"/>
     <col min="4" max="7" width="27" customWidth="1"/>
     <col min="8" max="8" width="15.1640625" customWidth="1"/>
-    <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="12" max="12" width="26.1640625" customWidth="1"/>
-    <col min="13" max="13" width="17.83203125" customWidth="1"/>
-    <col min="14" max="14" width="13.1640625" customWidth="1"/>
+    <col min="10" max="10" width="26.1640625" customWidth="1"/>
+    <col min="11" max="11" width="17.83203125" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
       </c>
       <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2">
-        <f>402.000456+153.1779</f>
-        <v>555.17835600000001</v>
+        <v>555</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1085,20 +1061,19 @@
         <v>65</v>
       </c>
       <c r="H2" s="2">
-        <v>1.2</v>
-      </c>
+        <v>1.5</v>
+      </c>
+      <c r="I2" s="3"/>
       <c r="J2" s="3"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K2" s="3"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>0.8</v>
@@ -1116,11 +1091,11 @@
         <v>0</v>
       </c>
       <c r="H3" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="O3" s="1"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+        <v>1.5</v>
+      </c>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1143,16 +1118,16 @@
         <v>0</v>
       </c>
       <c r="H4" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="O4" s="1"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+        <v>1.5</v>
+      </c>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5">
         <f>158.20187976+3.810456</f>
@@ -1168,27 +1143,27 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="H5" s="2">
         <v>1.8</v>
       </c>
-      <c r="K5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="O5" s="1"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6">
         <v>4.5</v>
       </c>
       <c r="D6">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1202,9 +1177,9 @@
       <c r="H6" s="2">
         <v>1.8</v>
       </c>
-      <c r="O6" s="1"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1229,14 +1204,14 @@
       <c r="H7" s="2">
         <v>1.8</v>
       </c>
-      <c r="O7" s="1"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8">
         <v>11</v>
@@ -1251,16 +1226,16 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="H8" s="2">
         <v>1.01</v>
       </c>
-      <c r="K8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="O8" s="1"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1277,7 +1252,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1285,14 +1260,14 @@
       <c r="H9" s="2">
         <v>1.01</v>
       </c>
-      <c r="O9" s="1"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10">
         <v>46.44885</v>
@@ -1312,16 +1287,16 @@
       <c r="H10" s="2">
         <v>14.27</v>
       </c>
-      <c r="K10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="O10" s="1"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11">
         <v>0.13128399999999998</v>
@@ -1341,9 +1316,9 @@
       <c r="H11" s="2">
         <v>14.27</v>
       </c>
-      <c r="O11" s="1"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1368,14 +1343,14 @@
       <c r="H12" s="2">
         <v>14.27</v>
       </c>
-      <c r="O12" s="1"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1395,11 +1370,11 @@
       <c r="H13" s="2">
         <v>14.27</v>
       </c>
-      <c r="O13" s="1"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
@@ -1423,9 +1398,9 @@
         <v>457.99206264078083</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
@@ -1449,12 +1424,12 @@
         <v>85.218116708716536</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16">
         <v>15.6</v>
@@ -1469,7 +1444,7 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <v>180</v>
+        <v>2160</v>
       </c>
       <c r="H16">
         <v>90</v>
@@ -1480,7 +1455,7 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17">
         <v>33.6</v>
@@ -1495,9 +1470,35 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>400</v>
+        <v>3500</v>
       </c>
       <c r="H17">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18">
+        <v>364</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>3500</v>
+      </c>
+      <c r="H18">
         <v>180</v>
       </c>
     </row>
@@ -1510,14 +1511,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1C53E1-07A4-9F44-81EF-FA7DBE0FC633}">
   <dimension ref="A1:W22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="23" width="11.83203125" customWidth="1"/>
+    <col min="2" max="16" width="11.83203125" customWidth="1"/>
+    <col min="17" max="17" width="14.83203125" customWidth="1"/>
+    <col min="18" max="23" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
@@ -1525,7 +1528,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
         <v>8</v>
@@ -1534,7 +1537,7 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
         <v>10</v>
@@ -1561,10 +1564,10 @@
         <v>18</v>
       </c>
       <c r="N1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" t="s">
         <v>36</v>
-      </c>
-      <c r="O1" t="s">
-        <v>37</v>
       </c>
       <c r="P1" t="s">
         <v>5</v>
@@ -1572,549 +1575,556 @@
       <c r="Q1" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
+      <c r="R1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8">
+        <v>33</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7">
         <v>0.1</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>0.8</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11">
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10">
         <v>0.1</v>
       </c>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11">
+      <c r="B3" s="9"/>
+      <c r="C3" s="10">
         <v>1</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="15">
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14">
         <v>1</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="11"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="7">
-        <v>0</v>
-      </c>
-      <c r="F5" s="8">
+        <v>34</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
         <v>0.1</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>0.9</v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="11"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10">
         <v>1</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="15">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="14">
         <v>1</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="7">
-        <v>0</v>
-      </c>
-      <c r="I8" s="9">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="6">
+        <v>0</v>
+      </c>
+      <c r="I8" s="8">
         <v>1</v>
       </c>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="15">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="14">
         <v>1</v>
       </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="7">
-        <v>0</v>
-      </c>
-      <c r="K10" s="8">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="6">
+        <v>0</v>
+      </c>
+      <c r="K10" s="7">
         <v>0.2</v>
       </c>
-      <c r="L10" s="8">
+      <c r="L10" s="7">
         <v>0.5</v>
       </c>
-      <c r="M10" s="9">
+      <c r="M10" s="8">
         <v>0.3</v>
       </c>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
-      <c r="U10" s="11"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="11">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="10">
         <v>1</v>
       </c>
-      <c r="L11" s="11"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
-      <c r="U11" s="11"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10">
         <v>1</v>
       </c>
-      <c r="M12" s="12"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="11"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="11"/>
-      <c r="W12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="15">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="14">
         <v>1</v>
       </c>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="11"/>
-      <c r="W13" s="11"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="10"/>
+      <c r="W13" s="10"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="7">
+        <v>35</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="6">
         <v>1</v>
       </c>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
-      <c r="U14" s="11"/>
-      <c r="V14" s="11"/>
-      <c r="W14" s="11"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="10"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="11">
+        <v>36</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="10">
         <v>1</v>
       </c>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11"/>
-      <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="11"/>
-      <c r="W15" s="11"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
+      <c r="W15" s="10"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="10">
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="9">
         <v>0.5</v>
       </c>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11">
+      <c r="O16" s="10"/>
+      <c r="P16" s="10">
         <v>0.5</v>
       </c>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="11"/>
-      <c r="S16" s="11"/>
-      <c r="T16" s="11"/>
-      <c r="U16" s="11"/>
-      <c r="V16" s="11"/>
-      <c r="W16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="15">
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="14">
         <v>1</v>
       </c>
-      <c r="R17" s="11"/>
-      <c r="S17" s="11"/>
-      <c r="T17" s="11"/>
-      <c r="U17" s="11"/>
-      <c r="V17" s="11"/>
-      <c r="W17" s="11"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="11"/>
-      <c r="S18" s="11"/>
-      <c r="T18" s="11"/>
-      <c r="U18" s="11"/>
-      <c r="V18" s="11"/>
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10">
+        <v>1</v>
+      </c>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="11"/>
-      <c r="S19" s="11"/>
-      <c r="T19" s="11"/>
-      <c r="U19" s="11"/>
-      <c r="V19" s="11"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="11"/>
-      <c r="S20" s="11"/>
-      <c r="T20" s="11"/>
-      <c r="U20" s="11"/>
-      <c r="V20" s="11"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="11"/>
-      <c r="S21" s="11"/>
-      <c r="T21" s="11"/>
-      <c r="U21" s="11"/>
-      <c r="V21" s="11"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
-      <c r="S22" s="11"/>
-      <c r="T22" s="11"/>
-      <c r="U22" s="11"/>
-      <c r="V22" s="11"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
mise à jour industrie
</commit_message>
<xml_diff>
--- a/Models/Prospective_conso/data/Hypotheses_Transport_1D.xlsx
+++ b/Models/Prospective_conso/data/Hypotheses_Transport_1D.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin.girard/Documents/Code/Etude/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E13D02B-AF35-8141-BBEB-836DFE5AFCCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE75FEC4-B9B8-7842-AC56-D0275D56E006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="5800" windowWidth="39920" windowHeight="21060" activeTab="3" xr2:uid="{F50204B1-83F4-DA42-A3C5-0BBDF8372860}"/>
+    <workbookView xWindow="23520" yWindow="1420" windowWidth="21460" windowHeight="21140" xr2:uid="{F50204B1-83F4-DA42-A3C5-0BBDF8372860}"/>
   </bookViews>
   <sheets>
     <sheet name="0D" sheetId="1" r:id="rId1"/>
     <sheet name="year" sheetId="6" r:id="rId2"/>
     <sheet name="year_Vecteur" sheetId="7" r:id="rId3"/>
     <sheet name="Categorie" sheetId="3" r:id="rId4"/>
-    <sheet name="retrofit_Transition" sheetId="8" r:id="rId5"/>
+    <sheet name="Categorie_year" sheetId="9" r:id="rId5"/>
+    <sheet name="retrofit_Transition" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="39">
   <si>
     <t>Nom</t>
   </si>
@@ -108,15 +109,6 @@
     <t>retrofit_change_total_proportion_Mds_voy_km</t>
   </si>
   <si>
-    <t>init_conso_unitaire_électrique</t>
-  </si>
-  <si>
-    <t>init_conso_unitaire_gaz</t>
-  </si>
-  <si>
-    <t>init_conso_unitaire_H2</t>
-  </si>
-  <si>
     <t>Vecteur</t>
   </si>
   <si>
@@ -126,15 +118,6 @@
     <t>H2</t>
   </si>
   <si>
-    <t>direct_emission</t>
-  </si>
-  <si>
-    <t>init_Vecteur</t>
-  </si>
-  <si>
-    <t>init_conso_unitaire_fuel</t>
-  </si>
-  <si>
     <t>fuel</t>
   </si>
   <si>
@@ -151,6 +134,27 @@
   </si>
   <si>
     <t>aerien_international</t>
+  </si>
+  <si>
+    <t>init_energy_need_per_Mds_voy_km</t>
+  </si>
+  <si>
+    <t>direct_emissions</t>
+  </si>
+  <si>
+    <t>indirect_emissions</t>
+  </si>
+  <si>
+    <t>conso_unitaire_gaz</t>
+  </si>
+  <si>
+    <t>conso_unitaire_H2</t>
+  </si>
+  <si>
+    <t>conso_unitaire_électrique</t>
+  </si>
+  <si>
+    <t>conso_unitaire_fuel</t>
   </si>
 </sst>
 </file>
@@ -161,7 +165,7 @@
     <numFmt numFmtId="44" formatCode="_ * #,##0.00_)\ &quot;€&quot;_ ;_ * \(#,##0.00\)\ &quot;€&quot;_ ;_ * &quot;-&quot;??_)\ &quot;€&quot;_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -191,11 +195,20 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -219,7 +232,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -308,26 +321,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top/>
       <bottom style="thin">
@@ -371,14 +364,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
@@ -694,9 +689,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{779B33ED-9EE9-BB48-B4CA-335F6E62A50A}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -714,7 +709,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B2">
@@ -722,7 +717,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="13" t="s">
         <v>20</v>
       </c>
       <c r="B3">
@@ -730,11 +725,19 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B4">
         <v>2050</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>
@@ -759,7 +762,7 @@
       <c r="A1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>22</v>
       </c>
     </row>
@@ -767,7 +770,7 @@
       <c r="A2">
         <v>2020</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="14">
         <v>0</v>
       </c>
     </row>
@@ -775,7 +778,7 @@
       <c r="A3">
         <v>2022</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="14">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
@@ -783,7 +786,7 @@
       <c r="A4">
         <v>2025</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="14">
         <v>0.1</v>
       </c>
     </row>
@@ -791,7 +794,7 @@
       <c r="A5">
         <v>2030</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="14">
         <v>0.35</v>
       </c>
     </row>
@@ -799,7 +802,7 @@
       <c r="A6">
         <v>2035</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="14">
         <v>0.7</v>
       </c>
     </row>
@@ -807,7 +810,7 @@
       <c r="A7">
         <v>2040</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="14">
         <v>0.85</v>
       </c>
     </row>
@@ -815,7 +818,7 @@
       <c r="A8">
         <v>2045</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="14">
         <v>0.95</v>
       </c>
     </row>
@@ -823,7 +826,7 @@
       <c r="A9">
         <v>2050</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="14">
         <v>1</v>
       </c>
     </row>
@@ -834,10 +837,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69DAC7EB-1A6F-3141-A691-43B6CE1216A5}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -845,20 +848,23 @@
     <col min="3" max="3" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>2020</v>
@@ -866,10 +872,13 @@
       <c r="C2" s="4">
         <v>264</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>2020</v>
@@ -877,10 +886,13 @@
       <c r="C3" s="5">
         <v>227</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>2020</v>
@@ -888,8 +900,11 @@
       <c r="C4">
         <v>120</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -899,10 +914,13 @@
       <c r="C5">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>2035</v>
@@ -910,10 +928,13 @@
       <c r="C6" s="4">
         <v>200</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>2035</v>
@@ -921,10 +942,13 @@
       <c r="C7" s="5">
         <v>75</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>2035</v>
@@ -932,8 +956,11 @@
       <c r="C8">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -943,10 +970,13 @@
       <c r="C9">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B10">
         <v>2050</v>
@@ -954,10 +984,13 @@
       <c r="C10" s="4">
         <v>160</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11">
         <v>2050</v>
@@ -965,10 +998,13 @@
       <c r="C11" s="5">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B12">
         <v>2050</v>
@@ -976,8 +1012,11 @@
       <c r="C12">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -986,6 +1025,9 @@
       </c>
       <c r="C13">
         <v>20</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -995,510 +1037,239 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9039F29E-2202-544B-A034-316D6E6A18F0}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.1640625" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
-    <col min="4" max="7" width="27" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" customWidth="1"/>
-    <col min="10" max="10" width="26.1640625" customWidth="1"/>
-    <col min="11" max="11" width="17.83203125" customWidth="1"/>
-    <col min="12" max="12" width="13.1640625" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2">
+        <v>27</v>
+      </c>
+      <c r="B2">
         <v>555</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>65</v>
-      </c>
-      <c r="H2" s="2">
+      <c r="C2" s="2">
         <v>1.5</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3">
+      <c r="B3">
         <v>0.8</v>
       </c>
-      <c r="D3">
-        <v>65</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
+      <c r="C3" s="2">
         <v>1.5</v>
       </c>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4">
+      <c r="B4">
         <v>1.2331949999999998</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>20</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2">
+      <c r="C4" s="2">
         <v>1.5</v>
       </c>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5">
+        <v>28</v>
+      </c>
+      <c r="B5">
         <f>158.20187976+3.810456</f>
         <v>162.01233575999998</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>85</v>
-      </c>
-      <c r="H5" s="2">
+      <c r="C5" s="2">
         <v>1.8</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6">
+      <c r="B6">
         <v>4.5</v>
       </c>
-      <c r="D6">
-        <v>85</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2">
+      <c r="C6" s="2">
         <v>1.8</v>
       </c>
-      <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7">
+      <c r="B7">
         <v>5.9867999999999998E-2</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>20</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
+      <c r="C7" s="2">
         <v>1.8</v>
       </c>
-      <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8">
+      <c r="B8">
         <v>11</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>50</v>
-      </c>
-      <c r="H8" s="2">
+      <c r="C8" s="2">
         <v>1.01</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9">
+      <c r="B9">
         <v>0.10691961</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>15</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2">
+      <c r="C9" s="2">
         <v>1.01</v>
       </c>
-      <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10">
+      <c r="B10">
         <v>46.44885</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>284</v>
-      </c>
-      <c r="H10" s="2">
+      <c r="C10" s="2">
         <v>14.27</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11">
+      <c r="B11">
         <v>0.13128399999999998</v>
       </c>
-      <c r="D11">
-        <v>280</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2">
+      <c r="C11" s="2">
         <v>14.27</v>
       </c>
-      <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12">
+      <c r="B12">
         <v>2.6256799999999997E-2</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>75</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12" s="2">
+      <c r="C12" s="2">
         <v>14.27</v>
       </c>
-      <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>200</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13" s="2">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
         <v>14.27</v>
       </c>
-      <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" t="s">
-        <v>3</v>
+        <v>29</v>
+      </c>
+      <c r="B14">
+        <v>63.46</v>
       </c>
       <c r="C14">
-        <v>63.46</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>1859</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
         <v>457.99206264078083</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>44.6</v>
       </c>
       <c r="C15">
-        <v>44.6</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>975</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
         <v>85.218116708716536</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
-      <c r="B16" t="s">
-        <v>32</v>
+      <c r="B16">
+        <v>15.6</v>
       </c>
       <c r="C16">
-        <v>15.6</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>2160</v>
-      </c>
-      <c r="H16">
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
-      <c r="B17" t="s">
-        <v>32</v>
+      <c r="B17">
+        <v>33.6</v>
       </c>
       <c r="C17">
-        <v>33.6</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>3500</v>
-      </c>
-      <c r="H17">
         <v>180</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="B18">
+        <v>364</v>
       </c>
       <c r="C18">
-        <v>364</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>3500</v>
-      </c>
-      <c r="H18">
         <v>180</v>
       </c>
     </row>
@@ -1508,11 +1279,386 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5F46D37-98FA-434F-944B-1D25EFC6D356}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C2" s="16">
+        <v>0</v>
+      </c>
+      <c r="D2" s="16">
+        <v>0</v>
+      </c>
+      <c r="E2" s="16">
+        <v>0</v>
+      </c>
+      <c r="F2" s="16">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C3" s="16">
+        <v>65</v>
+      </c>
+      <c r="D3" s="16">
+        <v>0</v>
+      </c>
+      <c r="E3" s="16">
+        <v>0</v>
+      </c>
+      <c r="F3" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C4" s="16">
+        <v>0</v>
+      </c>
+      <c r="D4" s="16">
+        <v>0</v>
+      </c>
+      <c r="E4" s="16">
+        <v>20</v>
+      </c>
+      <c r="F4" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C5" s="16">
+        <v>0</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0</v>
+      </c>
+      <c r="E5" s="16">
+        <v>0</v>
+      </c>
+      <c r="F5" s="16">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C6" s="16">
+        <v>85</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0</v>
+      </c>
+      <c r="E6" s="16">
+        <v>0</v>
+      </c>
+      <c r="F6" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C7" s="16">
+        <v>0</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0</v>
+      </c>
+      <c r="E7" s="16">
+        <v>20</v>
+      </c>
+      <c r="F7" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C8" s="16">
+        <v>0</v>
+      </c>
+      <c r="D8" s="16">
+        <v>0</v>
+      </c>
+      <c r="E8" s="16">
+        <v>0</v>
+      </c>
+      <c r="F8" s="16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C9" s="16">
+        <v>0</v>
+      </c>
+      <c r="D9" s="16">
+        <v>0</v>
+      </c>
+      <c r="E9" s="16">
+        <v>15</v>
+      </c>
+      <c r="F9" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C10" s="16">
+        <v>0</v>
+      </c>
+      <c r="D10" s="16">
+        <v>0</v>
+      </c>
+      <c r="E10" s="16">
+        <v>0</v>
+      </c>
+      <c r="F10" s="16">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C11" s="16">
+        <v>280</v>
+      </c>
+      <c r="D11" s="16">
+        <v>0</v>
+      </c>
+      <c r="E11" s="16">
+        <v>0</v>
+      </c>
+      <c r="F11" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C12" s="16">
+        <v>0</v>
+      </c>
+      <c r="D12" s="16">
+        <v>0</v>
+      </c>
+      <c r="E12" s="16">
+        <v>75</v>
+      </c>
+      <c r="F12" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C13" s="16">
+        <v>0</v>
+      </c>
+      <c r="D13" s="16">
+        <v>200</v>
+      </c>
+      <c r="E13" s="16">
+        <v>0</v>
+      </c>
+      <c r="F13" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C14" s="16">
+        <v>0</v>
+      </c>
+      <c r="D14" s="16">
+        <v>0</v>
+      </c>
+      <c r="E14" s="16">
+        <v>1859</v>
+      </c>
+      <c r="F14" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C15" s="16">
+        <v>0</v>
+      </c>
+      <c r="D15" s="16">
+        <v>0</v>
+      </c>
+      <c r="E15" s="16">
+        <v>975</v>
+      </c>
+      <c r="F15" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C16" s="16">
+        <v>0</v>
+      </c>
+      <c r="D16" s="16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="16">
+        <v>0</v>
+      </c>
+      <c r="F16" s="16">
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C17" s="16">
+        <v>0</v>
+      </c>
+      <c r="D17" s="16">
+        <v>0</v>
+      </c>
+      <c r="E17" s="16">
+        <v>0</v>
+      </c>
+      <c r="F17" s="16">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C18" s="16">
+        <v>0</v>
+      </c>
+      <c r="D18" s="16">
+        <v>0</v>
+      </c>
+      <c r="E18" s="16">
+        <v>0</v>
+      </c>
+      <c r="F18" s="16">
+        <v>3500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1C53E1-07A4-9F44-81EF-FA7DBE0FC633}">
   <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1528,7 +1674,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
         <v>8</v>
@@ -1537,7 +1683,7 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
         <v>10</v>
@@ -1564,10 +1710,10 @@
         <v>18</v>
       </c>
       <c r="N1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="O1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="P1" t="s">
         <v>5</v>
@@ -1576,7 +1722,7 @@
         <v>6</v>
       </c>
       <c r="R1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="S1" s="10"/>
       <c r="T1" s="10"/>
@@ -1586,31 +1732,59 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="6"/>
+        <v>27</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0</v>
+      </c>
       <c r="C2" s="7">
         <v>0.1</v>
       </c>
       <c r="D2" s="8">
         <v>0.8</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
+      <c r="E2" s="11">
+        <v>0</v>
+      </c>
+      <c r="F2" s="11">
+        <v>0</v>
+      </c>
+      <c r="G2" s="11">
+        <v>0</v>
+      </c>
+      <c r="H2" s="11">
+        <v>0</v>
+      </c>
+      <c r="I2" s="11">
+        <v>0</v>
+      </c>
+      <c r="J2" s="11">
+        <v>0</v>
+      </c>
+      <c r="K2" s="11">
+        <v>0</v>
+      </c>
+      <c r="L2" s="11">
+        <v>0</v>
+      </c>
+      <c r="M2" s="11">
+        <v>0</v>
+      </c>
+      <c r="N2" s="11">
+        <v>0</v>
+      </c>
       <c r="O2" s="10">
         <v>0.1</v>
       </c>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
+      <c r="P2" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="11">
+        <v>0</v>
+      </c>
+      <c r="R2" s="11">
+        <v>0</v>
+      </c>
       <c r="S2" s="10"/>
       <c r="T2" s="10"/>
       <c r="U2" s="10"/>
@@ -1621,25 +1795,57 @@
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="6">
+        <v>0</v>
+      </c>
       <c r="C3" s="10">
         <v>1</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
+      <c r="D3" s="11">
+        <v>0</v>
+      </c>
+      <c r="E3" s="11">
+        <v>0</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0</v>
+      </c>
+      <c r="G3" s="11">
+        <v>0</v>
+      </c>
+      <c r="H3" s="11">
+        <v>0</v>
+      </c>
+      <c r="I3" s="11">
+        <v>0</v>
+      </c>
+      <c r="J3" s="11">
+        <v>0</v>
+      </c>
+      <c r="K3" s="11">
+        <v>0</v>
+      </c>
+      <c r="L3" s="11">
+        <v>0</v>
+      </c>
+      <c r="M3" s="11">
+        <v>0</v>
+      </c>
+      <c r="N3" s="11">
+        <v>0</v>
+      </c>
+      <c r="O3" s="11">
+        <v>0</v>
+      </c>
+      <c r="P3" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="11">
+        <v>0</v>
+      </c>
+      <c r="R3" s="11">
+        <v>0</v>
+      </c>
       <c r="S3" s="10"/>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
@@ -1650,25 +1856,57 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14">
+      <c r="B4" s="6">
+        <v>0</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0</v>
+      </c>
+      <c r="D4" s="12">
         <v>1</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
+      <c r="E4" s="11">
+        <v>0</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11">
+        <v>0</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0</v>
+      </c>
+      <c r="J4" s="11">
+        <v>0</v>
+      </c>
+      <c r="K4" s="11">
+        <v>0</v>
+      </c>
+      <c r="L4" s="11">
+        <v>0</v>
+      </c>
+      <c r="M4" s="11">
+        <v>0</v>
+      </c>
+      <c r="N4" s="11">
+        <v>0</v>
+      </c>
+      <c r="O4" s="11">
+        <v>0</v>
+      </c>
+      <c r="P4" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="11">
+        <v>0</v>
+      </c>
+      <c r="R4" s="11">
+        <v>0</v>
+      </c>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
       <c r="U4" s="10"/>
@@ -1677,11 +1915,17 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
+        <v>28</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="11">
+        <v>0</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0</v>
+      </c>
       <c r="E5" s="6">
         <v>0</v>
       </c>
@@ -1691,17 +1935,39 @@
       <c r="G5" s="8">
         <v>0.9</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
+      <c r="H5" s="11">
+        <v>0</v>
+      </c>
+      <c r="I5" s="11">
+        <v>0</v>
+      </c>
+      <c r="J5" s="11">
+        <v>0</v>
+      </c>
+      <c r="K5" s="11">
+        <v>0</v>
+      </c>
+      <c r="L5" s="11">
+        <v>0</v>
+      </c>
+      <c r="M5" s="11">
+        <v>0</v>
+      </c>
+      <c r="N5" s="11">
+        <v>0</v>
+      </c>
+      <c r="O5" s="11">
+        <v>0</v>
+      </c>
+      <c r="P5" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="11">
+        <v>0</v>
+      </c>
+      <c r="R5" s="11">
+        <v>0</v>
+      </c>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
       <c r="U5" s="10"/>
@@ -1712,25 +1978,57 @@
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="9"/>
+      <c r="B6" s="6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="11">
+        <v>0</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0</v>
+      </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
+      <c r="G6" s="11">
+        <v>0</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0</v>
+      </c>
+      <c r="I6" s="11">
+        <v>0</v>
+      </c>
+      <c r="J6" s="11">
+        <v>0</v>
+      </c>
+      <c r="K6" s="11">
+        <v>0</v>
+      </c>
+      <c r="L6" s="11">
+        <v>0</v>
+      </c>
+      <c r="M6" s="11">
+        <v>0</v>
+      </c>
+      <c r="N6" s="11">
+        <v>0</v>
+      </c>
+      <c r="O6" s="11">
+        <v>0</v>
+      </c>
+      <c r="P6" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="11">
+        <v>0</v>
+      </c>
+      <c r="R6" s="11">
+        <v>0</v>
+      </c>
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
       <c r="U6" s="10"/>
@@ -1741,25 +2039,57 @@
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="14">
+      <c r="B7" s="6">
+        <v>0</v>
+      </c>
+      <c r="C7" s="11">
+        <v>0</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0</v>
+      </c>
+      <c r="E7" s="11">
+        <v>0</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0</v>
+      </c>
+      <c r="G7" s="12">
         <v>1</v>
       </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
+      <c r="H7" s="11">
+        <v>0</v>
+      </c>
+      <c r="I7" s="11">
+        <v>0</v>
+      </c>
+      <c r="J7" s="11">
+        <v>0</v>
+      </c>
+      <c r="K7" s="11">
+        <v>0</v>
+      </c>
+      <c r="L7" s="11">
+        <v>0</v>
+      </c>
+      <c r="M7" s="11">
+        <v>0</v>
+      </c>
+      <c r="N7" s="11">
+        <v>0</v>
+      </c>
+      <c r="O7" s="11">
+        <v>0</v>
+      </c>
+      <c r="P7" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="11">
+        <v>0</v>
+      </c>
+      <c r="R7" s="11">
+        <v>0</v>
+      </c>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
       <c r="U7" s="10"/>
@@ -1770,27 +2100,57 @@
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0</v>
+      </c>
+      <c r="D8" s="11">
+        <v>0</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0</v>
+      </c>
+      <c r="G8" s="11">
+        <v>0</v>
+      </c>
       <c r="H8" s="6">
         <v>0</v>
       </c>
       <c r="I8" s="8">
         <v>1</v>
       </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
+      <c r="J8" s="11">
+        <v>0</v>
+      </c>
+      <c r="K8" s="11">
+        <v>0</v>
+      </c>
+      <c r="L8" s="11">
+        <v>0</v>
+      </c>
+      <c r="M8" s="11">
+        <v>0</v>
+      </c>
+      <c r="N8" s="11">
+        <v>0</v>
+      </c>
+      <c r="O8" s="11">
+        <v>0</v>
+      </c>
+      <c r="P8" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="11">
+        <v>0</v>
+      </c>
+      <c r="R8" s="11">
+        <v>0</v>
+      </c>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
       <c r="U8" s="10"/>
@@ -1801,25 +2161,57 @@
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="14">
+      <c r="B9" s="6">
+        <v>0</v>
+      </c>
+      <c r="C9" s="11">
+        <v>0</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0</v>
+      </c>
+      <c r="I9" s="12">
         <v>1</v>
       </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
+      <c r="J9" s="11">
+        <v>0</v>
+      </c>
+      <c r="K9" s="11">
+        <v>0</v>
+      </c>
+      <c r="L9" s="11">
+        <v>0</v>
+      </c>
+      <c r="M9" s="11">
+        <v>0</v>
+      </c>
+      <c r="N9" s="11">
+        <v>0</v>
+      </c>
+      <c r="O9" s="11">
+        <v>0</v>
+      </c>
+      <c r="P9" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="11">
+        <v>0</v>
+      </c>
+      <c r="R9" s="11">
+        <v>0</v>
+      </c>
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
       <c r="U9" s="10"/>
@@ -1830,14 +2222,30 @@
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
+      <c r="B10" s="6">
+        <v>0</v>
+      </c>
+      <c r="C10" s="11">
+        <v>0</v>
+      </c>
+      <c r="D10" s="11">
+        <v>0</v>
+      </c>
+      <c r="E10" s="11">
+        <v>0</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0</v>
+      </c>
+      <c r="G10" s="11">
+        <v>0</v>
+      </c>
+      <c r="H10" s="11">
+        <v>0</v>
+      </c>
+      <c r="I10" s="11">
+        <v>0</v>
+      </c>
       <c r="J10" s="6">
         <v>0</v>
       </c>
@@ -1850,11 +2258,21 @@
       <c r="M10" s="8">
         <v>0.3</v>
       </c>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
+      <c r="N10" s="11">
+        <v>0</v>
+      </c>
+      <c r="O10" s="11">
+        <v>0</v>
+      </c>
+      <c r="P10" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="11">
+        <v>0</v>
+      </c>
+      <c r="R10" s="11">
+        <v>0</v>
+      </c>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
       <c r="U10" s="10"/>
@@ -1865,25 +2283,57 @@
       <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="9"/>
+      <c r="B11" s="6">
+        <v>0</v>
+      </c>
+      <c r="C11" s="11">
+        <v>0</v>
+      </c>
+      <c r="D11" s="11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="11">
+        <v>0</v>
+      </c>
+      <c r="F11" s="11">
+        <v>0</v>
+      </c>
+      <c r="G11" s="11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="11">
+        <v>0</v>
+      </c>
+      <c r="J11" s="11">
+        <v>0</v>
+      </c>
       <c r="K11" s="10">
         <v>1</v>
       </c>
-      <c r="L11" s="10"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
+      <c r="L11" s="11">
+        <v>0</v>
+      </c>
+      <c r="M11" s="11">
+        <v>0</v>
+      </c>
+      <c r="N11" s="11">
+        <v>0</v>
+      </c>
+      <c r="O11" s="11">
+        <v>0</v>
+      </c>
+      <c r="P11" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="11">
+        <v>0</v>
+      </c>
+      <c r="R11" s="11">
+        <v>0</v>
+      </c>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
       <c r="U11" s="10"/>
@@ -1894,25 +2344,57 @@
       <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="10"/>
+      <c r="B12" s="6">
+        <v>0</v>
+      </c>
+      <c r="C12" s="11">
+        <v>0</v>
+      </c>
+      <c r="D12" s="11">
+        <v>0</v>
+      </c>
+      <c r="E12" s="11">
+        <v>0</v>
+      </c>
+      <c r="F12" s="11">
+        <v>0</v>
+      </c>
+      <c r="G12" s="11">
+        <v>0</v>
+      </c>
+      <c r="H12" s="11">
+        <v>0</v>
+      </c>
+      <c r="I12" s="11">
+        <v>0</v>
+      </c>
+      <c r="J12" s="11">
+        <v>0</v>
+      </c>
+      <c r="K12" s="11">
+        <v>0</v>
+      </c>
       <c r="L12" s="10">
         <v>1</v>
       </c>
-      <c r="M12" s="11"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
+      <c r="M12" s="11">
+        <v>0</v>
+      </c>
+      <c r="N12" s="11">
+        <v>0</v>
+      </c>
+      <c r="O12" s="11">
+        <v>0</v>
+      </c>
+      <c r="P12" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="11">
+        <v>0</v>
+      </c>
+      <c r="R12" s="11">
+        <v>0</v>
+      </c>
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
       <c r="U12" s="10"/>
@@ -1923,25 +2405,57 @@
       <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="14">
+      <c r="B13" s="6">
+        <v>0</v>
+      </c>
+      <c r="C13" s="11">
+        <v>0</v>
+      </c>
+      <c r="D13" s="11">
+        <v>0</v>
+      </c>
+      <c r="E13" s="11">
+        <v>0</v>
+      </c>
+      <c r="F13" s="11">
+        <v>0</v>
+      </c>
+      <c r="G13" s="11">
+        <v>0</v>
+      </c>
+      <c r="H13" s="11">
+        <v>0</v>
+      </c>
+      <c r="I13" s="11">
+        <v>0</v>
+      </c>
+      <c r="J13" s="11">
+        <v>0</v>
+      </c>
+      <c r="K13" s="11">
+        <v>0</v>
+      </c>
+      <c r="L13" s="11">
+        <v>0</v>
+      </c>
+      <c r="M13" s="12">
         <v>1</v>
       </c>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
+      <c r="N13" s="11">
+        <v>0</v>
+      </c>
+      <c r="O13" s="11">
+        <v>0</v>
+      </c>
+      <c r="P13" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="11">
+        <v>0</v>
+      </c>
+      <c r="R13" s="11">
+        <v>0</v>
+      </c>
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
       <c r="U13" s="10"/>
@@ -1950,27 +2464,59 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
+        <v>29</v>
+      </c>
+      <c r="B14" s="6">
+        <v>0</v>
+      </c>
+      <c r="C14" s="11">
+        <v>0</v>
+      </c>
+      <c r="D14" s="11">
+        <v>0</v>
+      </c>
+      <c r="E14" s="11">
+        <v>0</v>
+      </c>
+      <c r="F14" s="11">
+        <v>0</v>
+      </c>
+      <c r="G14" s="11">
+        <v>0</v>
+      </c>
+      <c r="H14" s="11">
+        <v>0</v>
+      </c>
+      <c r="I14" s="11">
+        <v>0</v>
+      </c>
+      <c r="J14" s="11">
+        <v>0</v>
+      </c>
+      <c r="K14" s="11">
+        <v>0</v>
+      </c>
+      <c r="L14" s="11">
+        <v>0</v>
+      </c>
+      <c r="M14" s="11">
+        <v>0</v>
+      </c>
       <c r="N14" s="6">
         <v>1</v>
       </c>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="10"/>
+      <c r="O14" s="11">
+        <v>0</v>
+      </c>
+      <c r="P14" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="11">
+        <v>0</v>
+      </c>
+      <c r="R14" s="11">
+        <v>0</v>
+      </c>
       <c r="S14" s="10"/>
       <c r="T14" s="10"/>
       <c r="U14" s="10"/>
@@ -1979,27 +2525,59 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="9"/>
+        <v>30</v>
+      </c>
+      <c r="B15" s="6">
+        <v>0</v>
+      </c>
+      <c r="C15" s="11">
+        <v>0</v>
+      </c>
+      <c r="D15" s="11">
+        <v>0</v>
+      </c>
+      <c r="E15" s="11">
+        <v>0</v>
+      </c>
+      <c r="F15" s="11">
+        <v>0</v>
+      </c>
+      <c r="G15" s="11">
+        <v>0</v>
+      </c>
+      <c r="H15" s="11">
+        <v>0</v>
+      </c>
+      <c r="I15" s="11">
+        <v>0</v>
+      </c>
+      <c r="J15" s="11">
+        <v>0</v>
+      </c>
+      <c r="K15" s="11">
+        <v>0</v>
+      </c>
+      <c r="L15" s="11">
+        <v>0</v>
+      </c>
+      <c r="M15" s="11">
+        <v>0</v>
+      </c>
+      <c r="N15" s="11">
+        <v>0</v>
+      </c>
       <c r="O15" s="10">
         <v>1</v>
       </c>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="10"/>
+      <c r="P15" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="11">
+        <v>0</v>
+      </c>
+      <c r="R15" s="11">
+        <v>0</v>
+      </c>
       <c r="S15" s="10"/>
       <c r="T15" s="10"/>
       <c r="U15" s="10"/>
@@ -2010,27 +2588,57 @@
       <c r="A16" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
+      <c r="B16" s="6">
+        <v>0</v>
+      </c>
+      <c r="C16" s="11">
+        <v>0</v>
+      </c>
+      <c r="D16" s="11">
+        <v>0</v>
+      </c>
+      <c r="E16" s="11">
+        <v>0</v>
+      </c>
+      <c r="F16" s="11">
+        <v>0</v>
+      </c>
+      <c r="G16" s="11">
+        <v>0</v>
+      </c>
+      <c r="H16" s="11">
+        <v>0</v>
+      </c>
+      <c r="I16" s="11">
+        <v>0</v>
+      </c>
+      <c r="J16" s="11">
+        <v>0</v>
+      </c>
+      <c r="K16" s="11">
+        <v>0</v>
+      </c>
+      <c r="L16" s="11">
+        <v>0</v>
+      </c>
+      <c r="M16" s="11">
+        <v>0</v>
+      </c>
       <c r="N16" s="9">
         <v>0.5</v>
       </c>
-      <c r="O16" s="10"/>
+      <c r="O16" s="11">
+        <v>0</v>
+      </c>
       <c r="P16" s="10">
         <v>0.5</v>
       </c>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="10"/>
+      <c r="Q16" s="11">
+        <v>0</v>
+      </c>
+      <c r="R16" s="11">
+        <v>0</v>
+      </c>
       <c r="S16" s="10"/>
       <c r="T16" s="10"/>
       <c r="U16" s="10"/>
@@ -2041,25 +2649,57 @@
       <c r="A17" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="14">
+      <c r="B17" s="6">
+        <v>0</v>
+      </c>
+      <c r="C17" s="11">
+        <v>0</v>
+      </c>
+      <c r="D17" s="11">
+        <v>0</v>
+      </c>
+      <c r="E17" s="11">
+        <v>0</v>
+      </c>
+      <c r="F17" s="11">
+        <v>0</v>
+      </c>
+      <c r="G17" s="11">
+        <v>0</v>
+      </c>
+      <c r="H17" s="11">
+        <v>0</v>
+      </c>
+      <c r="I17" s="11">
+        <v>0</v>
+      </c>
+      <c r="J17" s="11">
+        <v>0</v>
+      </c>
+      <c r="K17" s="11">
+        <v>0</v>
+      </c>
+      <c r="L17" s="11">
+        <v>0</v>
+      </c>
+      <c r="M17" s="11">
+        <v>0</v>
+      </c>
+      <c r="N17" s="11">
+        <v>0</v>
+      </c>
+      <c r="O17" s="11">
+        <v>0</v>
+      </c>
+      <c r="P17" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="12">
         <v>1</v>
       </c>
-      <c r="R17" s="10"/>
+      <c r="R17" s="11">
+        <v>0</v>
+      </c>
       <c r="S17" s="10"/>
       <c r="T17" s="10"/>
       <c r="U17" s="10"/>
@@ -2068,12 +2708,56 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
+        <v>31</v>
+      </c>
+      <c r="B18" s="6">
+        <v>0</v>
+      </c>
+      <c r="C18" s="11">
+        <v>0</v>
+      </c>
+      <c r="D18" s="11">
+        <v>0</v>
+      </c>
+      <c r="E18" s="11">
+        <v>0</v>
+      </c>
+      <c r="F18" s="11">
+        <v>0</v>
+      </c>
+      <c r="G18" s="11">
+        <v>0</v>
+      </c>
+      <c r="H18" s="11">
+        <v>0</v>
+      </c>
+      <c r="I18" s="11">
+        <v>0</v>
+      </c>
+      <c r="J18" s="11">
+        <v>0</v>
+      </c>
+      <c r="K18" s="11">
+        <v>0</v>
+      </c>
+      <c r="L18" s="11">
+        <v>0</v>
+      </c>
+      <c r="M18" s="11">
+        <v>0</v>
+      </c>
+      <c r="N18" s="11">
+        <v>0</v>
+      </c>
+      <c r="O18" s="11">
+        <v>0</v>
+      </c>
+      <c r="P18" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="11">
+        <v>0</v>
+      </c>
       <c r="R18" s="10">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
new input file glass
</commit_message>
<xml_diff>
--- a/Models/Prospective_conso/data/Hypotheses_Transport_1D.xlsx
+++ b/Models/Prospective_conso/data/Hypotheses_Transport_1D.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin.girard/Documents/Code/Etude/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engie-my.sharepoint.com/personal/kv6345_engie_com/Documents/Documents/5-Python/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E13D02B-AF35-8141-BBEB-836DFE5AFCCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{8E13D02B-AF35-8141-BBEB-836DFE5AFCCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03A1ACFB-3A7F-4F58-9654-C4C37F1F85ED}"/>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="5800" windowWidth="39920" windowHeight="21060" activeTab="3" xr2:uid="{F50204B1-83F4-DA42-A3C5-0BBDF8372860}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{F50204B1-83F4-DA42-A3C5-0BBDF8372860}"/>
   </bookViews>
   <sheets>
     <sheet name="0D" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -158,8 +160,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_ * #,##0.00_)\ &quot;€&quot;_ ;_ * \(#,##0.00\)\ &quot;€&quot;_ ;_ * &quot;-&quot;??_)\ &quot;€&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_)\ &quot;€&quot;_ ;_ * \(#,##0.00\)\ &quot;€&quot;_ ;_ * &quot;-&quot;??_)\ &quot;€&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -349,11 +351,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -381,7 +383,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -398,7 +400,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -700,12 +702,12 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="20.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -713,7 +715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>19</v>
       </c>
@@ -721,7 +723,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>20</v>
       </c>
@@ -729,7 +731,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>21</v>
       </c>
@@ -750,12 +752,12 @@
       <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -763,7 +765,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2020</v>
       </c>
@@ -771,7 +773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2022</v>
       </c>
@@ -779,7 +781,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2025</v>
       </c>
@@ -787,7 +789,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2030</v>
       </c>
@@ -795,7 +797,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2035</v>
       </c>
@@ -803,7 +805,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2040</v>
       </c>
@@ -811,7 +813,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2045</v>
       </c>
@@ -819,7 +821,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2050</v>
       </c>
@@ -840,12 +842,12 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -856,7 +858,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -867,7 +869,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -878,7 +880,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -889,7 +891,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -900,7 +902,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -911,7 +913,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -922,7 +924,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -933,7 +935,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -944,7 +946,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -955,7 +957,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -966,7 +968,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -977,7 +979,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1001,18 +1003,18 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.19921875" customWidth="1"/>
     <col min="3" max="3" width="21.5" customWidth="1"/>
     <col min="4" max="7" width="27" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" customWidth="1"/>
-    <col min="10" max="10" width="26.1640625" customWidth="1"/>
-    <col min="11" max="11" width="17.83203125" customWidth="1"/>
-    <col min="12" max="12" width="13.1640625" customWidth="1"/>
+    <col min="8" max="8" width="15.19921875" customWidth="1"/>
+    <col min="10" max="10" width="26.19921875" customWidth="1"/>
+    <col min="11" max="11" width="17.796875" customWidth="1"/>
+    <col min="12" max="12" width="13.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1038,7 +1040,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1068,7 +1070,7 @@
       <c r="K2" s="3"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1095,7 +1097,7 @@
       </c>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1122,7 +1124,7 @@
       </c>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1152,7 +1154,7 @@
       <c r="K5" s="3"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1179,7 +1181,7 @@
       </c>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1206,7 +1208,7 @@
       </c>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1235,7 +1237,7 @@
       <c r="K8" s="3"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1262,7 +1264,7 @@
       </c>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1291,7 +1293,7 @@
       <c r="K10" s="3"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1318,7 +1320,7 @@
       </c>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1345,7 +1347,7 @@
       </c>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1372,7 +1374,7 @@
       </c>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1398,7 +1400,7 @@
         <v>457.99206264078083</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1424,7 +1426,7 @@
         <v>85.218116708716536</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1450,7 +1452,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1476,7 +1478,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -1515,15 +1517,15 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="16" width="11.83203125" customWidth="1"/>
-    <col min="17" max="17" width="14.83203125" customWidth="1"/>
-    <col min="18" max="23" width="11.83203125" customWidth="1"/>
+    <col min="2" max="16" width="11.796875" customWidth="1"/>
+    <col min="17" max="17" width="14.796875" customWidth="1"/>
+    <col min="18" max="23" width="11.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1584,7 +1586,7 @@
       <c r="V1" s="10"/>
       <c r="W1" s="10"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1617,7 +1619,7 @@
       <c r="V2" s="10"/>
       <c r="W2" s="10"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1646,7 +1648,7 @@
       <c r="V3" s="10"/>
       <c r="W3" s="10"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1675,7 +1677,7 @@
       <c r="V4" s="10"/>
       <c r="W4" s="10"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1708,7 +1710,7 @@
       <c r="V5" s="10"/>
       <c r="W5" s="10"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1737,7 +1739,7 @@
       <c r="V6" s="10"/>
       <c r="W6" s="10"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1766,7 +1768,7 @@
       <c r="V7" s="10"/>
       <c r="W7" s="10"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1797,7 +1799,7 @@
       <c r="V8" s="10"/>
       <c r="W8" s="10"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1826,7 +1828,7 @@
       <c r="V9" s="10"/>
       <c r="W9" s="10"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1861,7 +1863,7 @@
       <c r="V10" s="10"/>
       <c r="W10" s="10"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1890,7 +1892,7 @@
       <c r="V11" s="10"/>
       <c r="W11" s="10"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1919,7 +1921,7 @@
       <c r="V12" s="10"/>
       <c r="W12" s="10"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1948,7 +1950,7 @@
       <c r="V13" s="10"/>
       <c r="W13" s="10"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1977,7 +1979,7 @@
       <c r="V14" s="10"/>
       <c r="W14" s="10"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2006,7 +2008,7 @@
       <c r="V15" s="10"/>
       <c r="W15" s="10"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -2037,7 +2039,7 @@
       <c r="V16" s="10"/>
       <c r="W16" s="10"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -2066,7 +2068,7 @@
       <c r="V17" s="10"/>
       <c r="W17" s="10"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -2082,7 +2084,7 @@
       <c r="U18" s="10"/>
       <c r="V18" s="10"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
       <c r="P19" s="10"/>
@@ -2093,7 +2095,7 @@
       <c r="U19" s="10"/>
       <c r="V19" s="10"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="N20" s="10"/>
       <c r="O20" s="10"/>
       <c r="P20" s="10"/>
@@ -2104,7 +2106,7 @@
       <c r="U20" s="10"/>
       <c r="V20" s="10"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="N21" s="10"/>
       <c r="O21" s="10"/>
       <c r="P21" s="10"/>
@@ -2115,7 +2117,7 @@
       <c r="U21" s="10"/>
       <c r="V21" s="10"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="N22" s="10"/>
       <c r="O22" s="10"/>
       <c r="P22" s="10"/>

</xml_diff>

<commit_message>
removed all reference to match function
</commit_message>
<xml_diff>
--- a/Models/Prospective_conso/data/Hypotheses_Transport_1D.xlsx
+++ b/Models/Prospective_conso/data/Hypotheses_Transport_1D.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin.girard/Documents/Code/Etude/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE75FEC4-B9B8-7842-AC56-D0275D56E006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5199B5A-1998-154C-A976-45DDEEC9A95B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23520" yWindow="1420" windowWidth="21460" windowHeight="21140" xr2:uid="{F50204B1-83F4-DA42-A3C5-0BBDF8372860}"/>
+    <workbookView xWindow="140" yWindow="500" windowWidth="25140" windowHeight="14680" xr2:uid="{F50204B1-83F4-DA42-A3C5-0BBDF8372860}"/>
   </bookViews>
   <sheets>
     <sheet name="0D" sheetId="1" r:id="rId1"/>
@@ -692,7 +692,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -750,12 +750,13 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="2" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -840,7 +841,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1040,7 +1041,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1283,10 +1284,14 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
@@ -1657,8 +1662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1C53E1-07A4-9F44-81EF-FA7DBE0FC633}">
   <dimension ref="A1:W22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
ajout de la posibilité de réduire le besoin de transport
</commit_message>
<xml_diff>
--- a/Models/Prospective_conso/data/Hypotheses_Transport_1D.xlsx
+++ b/Models/Prospective_conso/data/Hypotheses_Transport_1D.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin.girard/Documents/Code/Etude/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5199B5A-1998-154C-A976-45DDEEC9A95B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7163F475-2EB5-884E-8190-DA2F31C74F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="500" windowWidth="25140" windowHeight="14680" xr2:uid="{F50204B1-83F4-DA42-A3C5-0BBDF8372860}"/>
+    <workbookView xWindow="13360" yWindow="4460" windowWidth="26280" windowHeight="17980" activeTab="4" xr2:uid="{F50204B1-83F4-DA42-A3C5-0BBDF8372860}"/>
   </bookViews>
   <sheets>
     <sheet name="0D" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="40">
   <si>
     <t>Nom</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>conso_unitaire_fuel</t>
+  </si>
+  <si>
+    <t>need_reduction</t>
   </si>
 </sst>
 </file>
@@ -691,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{779B33ED-9EE9-BB48-B4CA-335F6E62A50A}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -700,7 +703,7 @@
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -710,38 +713,39 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B2">
-        <v>0.1</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3">
-        <v>2020</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
-        <v>21</v>
+      <c r="A4" s="15" t="s">
+        <v>32</v>
       </c>
       <c r="B4">
-        <v>2050</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
-        <v>32</v>
+      <c r="A5" t="s">
+        <v>19</v>
       </c>
       <c r="B5">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -750,13 +754,13 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="44.33203125" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -841,7 +845,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1281,19 +1285,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5F46D37-98FA-434F-944B-1D25EFC6D356}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="17.6640625" customWidth="1"/>
     <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>2</v>
       </c>
@@ -1312,8 +1317,11 @@
       <c r="F1" s="16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>27</v>
       </c>
@@ -1332,8 +1340,11 @@
       <c r="F2" s="16">
         <v>65</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>8</v>
       </c>
@@ -1352,8 +1363,11 @@
       <c r="F3" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>9</v>
       </c>
@@ -1372,8 +1386,11 @@
       <c r="F4" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>28</v>
       </c>
@@ -1392,8 +1409,11 @@
       <c r="F5" s="16">
         <v>85</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
@@ -1412,8 +1432,11 @@
       <c r="F6" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>11</v>
       </c>
@@ -1432,8 +1455,11 @@
       <c r="F7" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>12</v>
       </c>
@@ -1452,8 +1478,11 @@
       <c r="F8" s="16">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
         <v>13</v>
       </c>
@@ -1472,8 +1501,11 @@
       <c r="F9" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>14</v>
       </c>
@@ -1492,8 +1524,11 @@
       <c r="F10" s="16">
         <v>284</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>15</v>
       </c>
@@ -1512,8 +1547,11 @@
       <c r="F11" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>16</v>
       </c>
@@ -1532,8 +1570,11 @@
       <c r="F12" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>18</v>
       </c>
@@ -1552,8 +1593,11 @@
       <c r="F13" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>29</v>
       </c>
@@ -1572,8 +1616,11 @@
       <c r="F14" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>30</v>
       </c>
@@ -1592,8 +1639,11 @@
       <c r="F15" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
         <v>5</v>
       </c>
@@ -1612,8 +1662,11 @@
       <c r="F16" s="16">
         <v>2160</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
         <v>6</v>
       </c>
@@ -1632,8 +1685,11 @@
       <c r="F17" s="16">
         <v>3500</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
         <v>31</v>
       </c>
@@ -1651,6 +1707,791 @@
       </c>
       <c r="F18" s="16">
         <v>3500</v>
+      </c>
+      <c r="G18" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C19" s="16">
+        <v>0</v>
+      </c>
+      <c r="D19" s="16">
+        <v>0</v>
+      </c>
+      <c r="E19" s="16">
+        <v>0</v>
+      </c>
+      <c r="F19" s="16">
+        <v>65</v>
+      </c>
+      <c r="G19" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C20" s="16">
+        <v>65</v>
+      </c>
+      <c r="D20" s="16">
+        <v>0</v>
+      </c>
+      <c r="E20" s="16">
+        <v>0</v>
+      </c>
+      <c r="F20" s="16">
+        <v>0</v>
+      </c>
+      <c r="G20" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C21" s="16">
+        <v>0</v>
+      </c>
+      <c r="D21" s="16">
+        <v>0</v>
+      </c>
+      <c r="E21" s="16">
+        <v>20</v>
+      </c>
+      <c r="F21" s="16">
+        <v>0</v>
+      </c>
+      <c r="G21" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C22" s="16">
+        <v>0</v>
+      </c>
+      <c r="D22" s="16">
+        <v>0</v>
+      </c>
+      <c r="E22" s="16">
+        <v>0</v>
+      </c>
+      <c r="F22" s="16">
+        <v>85</v>
+      </c>
+      <c r="G22" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C23" s="16">
+        <v>85</v>
+      </c>
+      <c r="D23" s="16">
+        <v>0</v>
+      </c>
+      <c r="E23" s="16">
+        <v>0</v>
+      </c>
+      <c r="F23" s="16">
+        <v>0</v>
+      </c>
+      <c r="G23" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C24" s="16">
+        <v>0</v>
+      </c>
+      <c r="D24" s="16">
+        <v>0</v>
+      </c>
+      <c r="E24" s="16">
+        <v>20</v>
+      </c>
+      <c r="F24" s="16">
+        <v>0</v>
+      </c>
+      <c r="G24" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C25" s="16">
+        <v>0</v>
+      </c>
+      <c r="D25" s="16">
+        <v>0</v>
+      </c>
+      <c r="E25" s="16">
+        <v>0</v>
+      </c>
+      <c r="F25" s="16">
+        <v>50</v>
+      </c>
+      <c r="G25" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C26" s="16">
+        <v>0</v>
+      </c>
+      <c r="D26" s="16">
+        <v>0</v>
+      </c>
+      <c r="E26" s="16">
+        <v>15</v>
+      </c>
+      <c r="F26" s="16">
+        <v>0</v>
+      </c>
+      <c r="G26" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C27" s="16">
+        <v>0</v>
+      </c>
+      <c r="D27" s="16">
+        <v>0</v>
+      </c>
+      <c r="E27" s="16">
+        <v>0</v>
+      </c>
+      <c r="F27" s="16">
+        <v>284</v>
+      </c>
+      <c r="G27" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C28" s="16">
+        <v>280</v>
+      </c>
+      <c r="D28" s="16">
+        <v>0</v>
+      </c>
+      <c r="E28" s="16">
+        <v>0</v>
+      </c>
+      <c r="F28" s="16">
+        <v>0</v>
+      </c>
+      <c r="G28" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C29" s="16">
+        <v>0</v>
+      </c>
+      <c r="D29" s="16">
+        <v>0</v>
+      </c>
+      <c r="E29" s="16">
+        <v>75</v>
+      </c>
+      <c r="F29" s="16">
+        <v>0</v>
+      </c>
+      <c r="G29" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C30" s="16">
+        <v>0</v>
+      </c>
+      <c r="D30" s="16">
+        <v>200</v>
+      </c>
+      <c r="E30" s="16">
+        <v>0</v>
+      </c>
+      <c r="F30" s="16">
+        <v>0</v>
+      </c>
+      <c r="G30" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C31" s="16">
+        <v>0</v>
+      </c>
+      <c r="D31" s="16">
+        <v>0</v>
+      </c>
+      <c r="E31" s="16">
+        <v>1859</v>
+      </c>
+      <c r="F31" s="16">
+        <v>0</v>
+      </c>
+      <c r="G31" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C32" s="16">
+        <v>0</v>
+      </c>
+      <c r="D32" s="16">
+        <v>0</v>
+      </c>
+      <c r="E32" s="16">
+        <v>975</v>
+      </c>
+      <c r="F32" s="16">
+        <v>0</v>
+      </c>
+      <c r="G32" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C33" s="16">
+        <v>0</v>
+      </c>
+      <c r="D33" s="16">
+        <v>0</v>
+      </c>
+      <c r="E33" s="16">
+        <v>0</v>
+      </c>
+      <c r="F33" s="16">
+        <v>2160</v>
+      </c>
+      <c r="G33">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C34" s="16">
+        <v>0</v>
+      </c>
+      <c r="D34" s="16">
+        <v>0</v>
+      </c>
+      <c r="E34" s="16">
+        <v>0</v>
+      </c>
+      <c r="F34" s="16">
+        <v>3500</v>
+      </c>
+      <c r="G34" s="16">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C35" s="16">
+        <v>0</v>
+      </c>
+      <c r="D35" s="16">
+        <v>0</v>
+      </c>
+      <c r="E35" s="16">
+        <v>0</v>
+      </c>
+      <c r="F35" s="16">
+        <v>3500</v>
+      </c>
+      <c r="G35" s="16">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C36" s="16">
+        <v>0</v>
+      </c>
+      <c r="D36" s="16">
+        <v>0</v>
+      </c>
+      <c r="E36" s="16">
+        <v>0</v>
+      </c>
+      <c r="F36" s="16">
+        <v>65</v>
+      </c>
+      <c r="G36" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C37" s="16">
+        <v>65</v>
+      </c>
+      <c r="D37" s="16">
+        <v>0</v>
+      </c>
+      <c r="E37" s="16">
+        <v>0</v>
+      </c>
+      <c r="F37" s="16">
+        <v>0</v>
+      </c>
+      <c r="G37" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C38" s="16">
+        <v>0</v>
+      </c>
+      <c r="D38" s="16">
+        <v>0</v>
+      </c>
+      <c r="E38" s="16">
+        <v>20</v>
+      </c>
+      <c r="F38" s="16">
+        <v>0</v>
+      </c>
+      <c r="G38" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B39" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C39" s="16">
+        <v>0</v>
+      </c>
+      <c r="D39" s="16">
+        <v>0</v>
+      </c>
+      <c r="E39" s="16">
+        <v>0</v>
+      </c>
+      <c r="F39" s="16">
+        <v>85</v>
+      </c>
+      <c r="G39" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C40" s="16">
+        <v>85</v>
+      </c>
+      <c r="D40" s="16">
+        <v>0</v>
+      </c>
+      <c r="E40" s="16">
+        <v>0</v>
+      </c>
+      <c r="F40" s="16">
+        <v>0</v>
+      </c>
+      <c r="G40" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C41" s="16">
+        <v>0</v>
+      </c>
+      <c r="D41" s="16">
+        <v>0</v>
+      </c>
+      <c r="E41" s="16">
+        <v>20</v>
+      </c>
+      <c r="F41" s="16">
+        <v>0</v>
+      </c>
+      <c r="G41" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C42" s="16">
+        <v>0</v>
+      </c>
+      <c r="D42" s="16">
+        <v>0</v>
+      </c>
+      <c r="E42" s="16">
+        <v>0</v>
+      </c>
+      <c r="F42" s="16">
+        <v>50</v>
+      </c>
+      <c r="G42" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C43" s="16">
+        <v>0</v>
+      </c>
+      <c r="D43" s="16">
+        <v>0</v>
+      </c>
+      <c r="E43" s="16">
+        <v>15</v>
+      </c>
+      <c r="F43" s="16">
+        <v>0</v>
+      </c>
+      <c r="G43" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C44" s="16">
+        <v>0</v>
+      </c>
+      <c r="D44" s="16">
+        <v>0</v>
+      </c>
+      <c r="E44" s="16">
+        <v>0</v>
+      </c>
+      <c r="F44" s="16">
+        <v>284</v>
+      </c>
+      <c r="G44" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C45" s="16">
+        <v>280</v>
+      </c>
+      <c r="D45" s="16">
+        <v>0</v>
+      </c>
+      <c r="E45" s="16">
+        <v>0</v>
+      </c>
+      <c r="F45" s="16">
+        <v>0</v>
+      </c>
+      <c r="G45" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C46" s="16">
+        <v>0</v>
+      </c>
+      <c r="D46" s="16">
+        <v>0</v>
+      </c>
+      <c r="E46" s="16">
+        <v>75</v>
+      </c>
+      <c r="F46" s="16">
+        <v>0</v>
+      </c>
+      <c r="G46" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C47" s="16">
+        <v>0</v>
+      </c>
+      <c r="D47" s="16">
+        <v>200</v>
+      </c>
+      <c r="E47" s="16">
+        <v>0</v>
+      </c>
+      <c r="F47" s="16">
+        <v>0</v>
+      </c>
+      <c r="G47" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B48" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C48" s="16">
+        <v>0</v>
+      </c>
+      <c r="D48" s="16">
+        <v>0</v>
+      </c>
+      <c r="E48" s="16">
+        <v>1859</v>
+      </c>
+      <c r="F48" s="16">
+        <v>0</v>
+      </c>
+      <c r="G48" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B49" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C49" s="16">
+        <v>0</v>
+      </c>
+      <c r="D49" s="16">
+        <v>0</v>
+      </c>
+      <c r="E49" s="16">
+        <v>975</v>
+      </c>
+      <c r="F49" s="16">
+        <v>0</v>
+      </c>
+      <c r="G49" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C50" s="16">
+        <v>0</v>
+      </c>
+      <c r="D50" s="16">
+        <v>0</v>
+      </c>
+      <c r="E50" s="16">
+        <v>0</v>
+      </c>
+      <c r="F50" s="16">
+        <v>2160</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C51" s="16">
+        <v>0</v>
+      </c>
+      <c r="D51" s="16">
+        <v>0</v>
+      </c>
+      <c r="E51" s="16">
+        <v>0</v>
+      </c>
+      <c r="F51" s="16">
+        <v>3500</v>
+      </c>
+      <c r="G51" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C52" s="16">
+        <v>0</v>
+      </c>
+      <c r="D52" s="16">
+        <v>0</v>
+      </c>
+      <c r="E52" s="16">
+        <v>0</v>
+      </c>
+      <c r="F52" s="16">
+        <v>3500</v>
+      </c>
+      <c r="G52" s="16">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>